<commit_message>
fix images and finish 1414
</commit_message>
<xml_diff>
--- a/excel/6/1414 N Oakes - Model.xlsx
+++ b/excel/6/1414 N Oakes - Model.xlsx
@@ -741,124 +741,124 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="1">
-                  <c:v>1.2576806818270878</c:v>
+                  <c:v>-3.8024839645304842E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68300881184536066</c:v>
+                  <c:v>-6.8386037690388599E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47816356310282204</c:v>
+                  <c:v>4.293684736192298E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37307616419540857</c:v>
+                  <c:v>1.0016804336968057E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30915871787414301</c:v>
+                  <c:v>1.3507749260033675E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26619037993170008</c:v>
+                  <c:v>1.5863017795791436E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23532926922846664</c:v>
+                  <c:v>1.756207130794827E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21209547273628249</c:v>
+                  <c:v>1.8847838540452012E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.20869010313109818</c:v>
+                  <c:v>3.4570162279247744E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19248093899912688</c:v>
+                  <c:v>3.3697399979837901E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.17920299234450995</c:v>
+                  <c:v>3.2988785143403289E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16812981058863588</c:v>
+                  <c:v>3.2403733186473008E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.15875661673471408</c:v>
+                  <c:v>3.191404380315481E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.15072174646537706</c:v>
+                  <c:v>3.1499511880656937E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.14375928546062383</c:v>
+                  <c:v>3.1145281481574093E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13766934848231013</c:v>
+                  <c:v>3.0840185421059419E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.13229878188768052</c:v>
+                  <c:v>3.0575667171113503E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.12752826022473179</c:v>
+                  <c:v>3.0345059983922843E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12326343452749274</c:v>
+                  <c:v>3.0143092372106151E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.1194287218429585</c:v>
+                  <c:v>2.9965541147059092E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.11596286008974531</c:v>
+                  <c:v>2.9808983081378467E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.1128156692995725</c:v>
+                  <c:v>2.9670613968504379E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.10994565379980616</c:v>
+                  <c:v>2.9548114663392747E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.10731820116278989</c:v>
+                  <c:v>2.9439550462907051E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.10490421154690296</c:v>
+                  <c:v>2.9343294531030073E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.10267904203456556</c:v>
+                  <c:v>2.9257968922122377E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.10062168462705127</c:v>
+                  <c:v>2.9182398657987451E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9.8714119706590192E-2</c:v>
+                  <c:v>2.9115575607861103E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9.6940802768885365E-2</c:v>
+                  <c:v>2.9056629813906405E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>9.5288253441250331E-2</c:v>
+                  <c:v>2.9004806531183883E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.3390114355828243E-2</c:v>
+                  <c:v>1.8604838282208557E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.3390114355828188E-2</c:v>
+                  <c:v>1.8604838282208505E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.3390114355828368E-2</c:v>
+                  <c:v>1.8604838282208665E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3390114355828326E-2</c:v>
+                  <c:v>1.860483828220864E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.3390114355828243E-2</c:v>
+                  <c:v>1.8604838282208554E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.3390114355828326E-2</c:v>
+                  <c:v>1.8604838282208637E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.3390114355828313E-2</c:v>
+                  <c:v>1.860483828220863E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8.3390114355828368E-2</c:v>
+                  <c:v>1.8604838282208686E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.3390114355828257E-2</c:v>
+                  <c:v>1.8604838282208581E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8.3390114355828229E-2</c:v>
+                  <c:v>1.8604838282208543E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1347,124 +1347,124 @@
                   <c:v>-76301.460000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6582.8315999999986</c:v>
+                  <c:v>-19817.168400000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7235.5257479999982</c:v>
+                  <c:v>-19956.474252</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7907.8007204399992</c:v>
+                  <c:v>-20099.95927956</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8600.243942053201</c:v>
+                  <c:v>-20247.748857946801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9313.4604603147964</c:v>
+                  <c:v>-20399.972123685206</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10048.073474124245</c:v>
+                  <c:v>-20556.762087395764</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10804.724878347977</c:v>
+                  <c:v>-20718.255750017634</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11584.075824698415</c:v>
+                  <c:v>-20884.594222518164</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15212.80729943937</c:v>
+                  <c:v>-18229.92284919371</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16039.620718422546</c:v>
+                  <c:v>-18406.391334669523</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16891.238539975224</c:v>
+                  <c:v>-18588.153874709606</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17768.404896174481</c:v>
+                  <c:v>-18775.369290950897</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18671.886243059715</c:v>
+                  <c:v>-18968.201169679422</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19602.472030351506</c:v>
+                  <c:v>-19166.818004769804</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20560.975391262054</c:v>
+                  <c:v>-19371.393344912904</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21548.233852999918</c:v>
+                  <c:v>-19582.105945260286</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22565.110068589922</c:v>
+                  <c:v>-19799.139923618095</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23612.492570647613</c:v>
+                  <c:v>-20022.68492132664</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24691.296547767044</c:v>
+                  <c:v>-20252.936268966441</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25802.464644200059</c:v>
+                  <c:v>-20490.095157035434</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26946.967783526066</c:v>
+                  <c:v>-20734.368811746495</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28125.806017031849</c:v>
+                  <c:v>-20985.970676098892</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>29340.00939754281</c:v>
+                  <c:v>-21245.120596381857</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30590.638879469097</c:v>
+                  <c:v>-21512.045014273313</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>31878.787245853171</c:v>
+                  <c:v>-21786.977164701515</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>33205.580063228772</c:v>
+                  <c:v>-22070.157279642561</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34572.176665125633</c:v>
+                  <c:v>-22361.832798031835</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35979.771165079408</c:v>
+                  <c:v>-22662.258581972794</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>37429.593500031784</c:v>
+                  <c:v>-22971.697139431977</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>38922.910505032734</c:v>
+                  <c:v>-23290.418853614938</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>52808.667020183719</c:v>
+                  <c:v>-11271.062219223384</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>54392.927030789237</c:v>
+                  <c:v>-11609.194085800087</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>56024.714841712921</c:v>
+                  <c:v>-11957.469908374091</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>57705.456286964305</c:v>
+                  <c:v>-12316.194005625313</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>59436.61997557323</c:v>
+                  <c:v>-12685.679825794072</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>61219.71857484043</c:v>
+                  <c:v>-13066.250220567894</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>63056.310132085644</c:v>
+                  <c:v>-13458.237727184931</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>64947.999436048223</c:v>
+                  <c:v>-13861.98485900048</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>66896.43941912966</c:v>
+                  <c:v>-14277.844404770494</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>68903.332601703558</c:v>
+                  <c:v>-14706.179736913611</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3115,8 +3115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C96533-4FC3-8F4F-BA09-1D518A28119D}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3250,7 +3250,7 @@
         <v>-386.96070000000003</v>
       </c>
       <c r="F3" s="5">
-        <v>2200</v>
+        <v>0</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
@@ -3277,15 +3277,15 @@
       </c>
       <c r="M3" s="16">
         <f>L3-L2+12*(C3+D3+E3+F3)+G3</f>
-        <v>25625.243892226914</v>
+        <v>-774.75610777308611</v>
       </c>
       <c r="N3" s="17">
         <f>M3/L2</f>
-        <v>1.2576806818270878</v>
+        <v>-3.8024839645304842E-2</v>
       </c>
       <c r="O3" s="16">
         <f>12*(C3+D3+E3+F3)+G3</f>
-        <v>6582.8315999999986</v>
+        <v>-19817.168400000002</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="F4" s="5">
         <f>F3*(1+B4)</f>
-        <v>2266</v>
+        <v>0</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -3334,15 +3334,15 @@
       </c>
       <c r="M4" s="16">
         <f>L4-L3+12*(C4+D4+E4+F4)+G4</f>
-        <v>26922.439935732618</v>
+        <v>-269.56006426738168</v>
       </c>
       <c r="N4" s="17">
         <f>M4/L3</f>
-        <v>0.68300881184536066</v>
+        <v>-6.8386037690388599E-3</v>
       </c>
       <c r="O4" s="16">
         <f t="shared" ref="O4:O66" si="6">12*(C4+D4+E4+F4)+G4</f>
-        <v>7235.5257479999982</v>
+        <v>-19956.474252</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -3364,7 +3364,7 @@
       </c>
       <c r="F5" s="5">
         <f t="shared" ref="F5:F66" si="7">F4*(1+B5)</f>
-        <v>2333.98</v>
+        <v>0</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -3391,15 +3391,15 @@
       </c>
       <c r="M5" s="16">
         <f t="shared" ref="M5:M66" si="8">L5-L4+12*(C5+D5+E5+F5)+G5</f>
-        <v>28261.535344449927</v>
+        <v>253.77534444992853</v>
       </c>
       <c r="N5" s="17">
         <f t="shared" ref="N5:N66" si="9">M5/L4</f>
-        <v>0.47816356310282204</v>
+        <v>4.293684736192298E-3</v>
       </c>
       <c r="O5" s="16">
         <f t="shared" si="6"/>
-        <v>7907.8007204399992</v>
+        <v>-20099.95927956</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="7"/>
-        <v>2403.9994000000002</v>
+        <v>0</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -3448,15 +3448,15 @@
       </c>
       <c r="M6" s="16">
         <f t="shared" si="8"/>
-        <v>29643.908651073318</v>
+        <v>795.91585107331412</v>
       </c>
       <c r="N6" s="17">
         <f t="shared" si="9"/>
-        <v>0.37307616419540857</v>
+        <v>1.0016804336968057E-2</v>
       </c>
       <c r="O6" s="16">
         <f t="shared" si="6"/>
-        <v>8600.243942053201</v>
+        <v>-20247.748857946801</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -3478,7 +3478,7 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="7"/>
-        <v>2476.1193820000003</v>
+        <v>0</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -3505,15 +3505,15 @@
       </c>
       <c r="M7" s="16">
         <f t="shared" si="8"/>
-        <v>31070.984696482519</v>
+        <v>1357.5521124825173</v>
       </c>
       <c r="N7" s="17">
         <f t="shared" si="9"/>
-        <v>0.30915871787414301</v>
+        <v>1.3507749260033675E-2</v>
       </c>
       <c r="O7" s="16">
         <f t="shared" si="6"/>
-        <v>9313.4604603147964</v>
+        <v>-20399.972123685206</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="7"/>
-        <v>2550.4029634600006</v>
+        <v>0</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -3562,15 +3562,15 @@
       </c>
       <c r="M8" s="16">
         <f t="shared" si="8"/>
-        <v>32544.236220749906</v>
+        <v>1939.4006592298974</v>
       </c>
       <c r="N8" s="17">
         <f t="shared" si="9"/>
-        <v>0.26619037993170008</v>
+        <v>1.5863017795791436E-2</v>
       </c>
       <c r="O8" s="16">
         <f t="shared" si="6"/>
-        <v>10048.073474124245</v>
+        <v>-20556.762087395764</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="7"/>
-        <v>2626.9150523638009</v>
+        <v>0</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -3620,15 +3620,15 @@
       </c>
       <c r="M9" s="16">
         <f t="shared" si="8"/>
-        <v>34065.185510096635</v>
+        <v>2542.2048817310279</v>
       </c>
       <c r="N9" s="17">
         <f t="shared" si="9"/>
-        <v>0.23532926922846664</v>
+        <v>1.756207130794827E-2</v>
       </c>
       <c r="O9" s="16">
         <f t="shared" si="6"/>
-        <v>10804.724878347977</v>
+        <v>-20718.255750017634</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="7"/>
-        <v>2705.722503934715</v>
+        <v>0</v>
       </c>
       <c r="G10" s="5">
         <v>0</v>
@@ -3678,15 +3678,15 @@
       </c>
       <c r="M10" s="16">
         <f t="shared" si="8"/>
-        <v>35635.406101811721</v>
+        <v>3166.7360545951378</v>
       </c>
       <c r="N10" s="17">
         <f t="shared" si="9"/>
-        <v>0.21209547273628249</v>
+        <v>1.8847838540452012E-2</v>
       </c>
       <c r="O10" s="16">
         <f t="shared" si="6"/>
-        <v>11584.075824698415</v>
+        <v>-20884.594222518164</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="7"/>
-        <v>2786.8941790527565</v>
+        <v>0</v>
       </c>
       <c r="G11" s="5">
         <v>0</v>
@@ -3736,15 +3736,15 @@
       </c>
       <c r="M11" s="16">
         <f t="shared" si="8"/>
-        <v>40082.524549223992</v>
+        <v>6639.7944005909085</v>
       </c>
       <c r="N11" s="17">
         <f t="shared" si="9"/>
-        <v>0.20869010313109818</v>
+        <v>3.4570162279247744E-2</v>
       </c>
       <c r="O11" s="16">
         <f t="shared" si="6"/>
-        <v>15212.80729943937</v>
+        <v>-18229.92284919371</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -3767,7 +3767,7 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="7"/>
-        <v>2870.501004424339</v>
+        <v>0</v>
       </c>
       <c r="G12" s="5">
         <v>0</v>
@@ -3794,15 +3794,15 @@
       </c>
       <c r="M12" s="16">
         <f t="shared" si="8"/>
-        <v>41756.222248887963</v>
+        <v>7310.2101957958912</v>
       </c>
       <c r="N12" s="17">
         <f t="shared" si="9"/>
-        <v>0.19248093899912688</v>
+        <v>3.3697399979837901E-2</v>
       </c>
       <c r="O12" s="16">
         <f t="shared" si="6"/>
-        <v>16039.620718422546</v>
+        <v>-18406.391334669523</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="7"/>
-        <v>2956.6160345570693</v>
+        <v>0</v>
       </c>
       <c r="G13" s="5">
         <v>0</v>
@@ -3852,15 +3852,15 @@
       </c>
       <c r="M13" s="16">
         <f t="shared" si="8"/>
-        <v>43484.237332229008</v>
+        <v>8004.8449175441783</v>
       </c>
       <c r="N13" s="17">
         <f t="shared" si="9"/>
-        <v>0.17920299234450995</v>
+        <v>3.2988785143403289E-2</v>
       </c>
       <c r="O13" s="16">
         <f t="shared" si="6"/>
-        <v>16891.238539975224</v>
+        <v>-18588.153874709606</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -3883,7 +3883,7 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="7"/>
-        <v>3045.3145155937814</v>
+        <v>0</v>
       </c>
       <c r="G14" s="5">
         <v>0</v>
@@ -3910,15 +3910,15 @@
       </c>
       <c r="M14" s="16">
         <f t="shared" si="8"/>
-        <v>45268.366623976137</v>
+        <v>8724.5924368507549</v>
       </c>
       <c r="N14" s="17">
         <f t="shared" si="9"/>
-        <v>0.16812981058863588</v>
+        <v>3.2403733186473008E-2</v>
       </c>
       <c r="O14" s="16">
         <f t="shared" si="6"/>
-        <v>17768.404896174481</v>
+        <v>-18775.369290950897</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="7"/>
-        <v>3136.6739510615948</v>
+        <v>0</v>
       </c>
       <c r="G15" s="5">
         <v>0</v>
@@ -3968,15 +3968,15 @@
       </c>
       <c r="M15" s="16">
         <f t="shared" si="8"/>
-        <v>47110.467669791258</v>
+        <v>9470.380257052122</v>
       </c>
       <c r="N15" s="17">
         <f t="shared" si="9"/>
-        <v>0.15875661673471408</v>
+        <v>3.191404380315481E-2</v>
       </c>
       <c r="O15" s="16">
         <f t="shared" si="6"/>
-        <v>18671.886243059715</v>
+        <v>-18968.201169679422</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -3999,7 +3999,7 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="7"/>
-        <v>3230.7741695934428</v>
+        <v>0</v>
       </c>
       <c r="G16" s="5">
         <v>0</v>
@@ -4026,15 +4026,15 @@
       </c>
       <c r="M16" s="16">
         <f t="shared" si="8"/>
-        <v>49012.460835599268</v>
+        <v>10243.170800477958</v>
       </c>
       <c r="N16" s="17">
         <f t="shared" si="9"/>
-        <v>0.15072174646537706</v>
+        <v>3.1499511880656937E-2</v>
       </c>
       <c r="O16" s="16">
         <f t="shared" si="6"/>
-        <v>19602.472030351506</v>
+        <v>-19166.818004769804</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -4057,7 +4057,7 @@
       </c>
       <c r="F17" s="5">
         <f t="shared" si="7"/>
-        <v>3327.6973946812464</v>
+        <v>0</v>
       </c>
       <c r="G17" s="5">
         <v>0</v>
@@ -4084,15 +4084,15 @@
       </c>
       <c r="M17" s="16">
         <f t="shared" si="8"/>
-        <v>50976.331481212881</v>
+        <v>11043.962745037927</v>
       </c>
       <c r="N17" s="17">
         <f t="shared" si="9"/>
-        <v>0.14375928546062383</v>
+        <v>3.1145281481574093E-2</v>
       </c>
       <c r="O17" s="16">
         <f t="shared" si="6"/>
-        <v>20560.975391262054</v>
+        <v>-19371.393344912904</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -4115,7 +4115,7 @@
       </c>
       <c r="F18" s="5">
         <f t="shared" si="7"/>
-        <v>3427.5283165216838</v>
+        <v>0</v>
       </c>
       <c r="G18" s="5">
         <v>0</v>
@@ -4142,15 +4142,15 @@
       </c>
       <c r="M18" s="16">
         <f t="shared" si="8"/>
-        <v>53004.132210939184</v>
+        <v>11873.79241267898</v>
       </c>
       <c r="N18" s="17">
         <f t="shared" si="9"/>
-        <v>0.13766934848231013</v>
+        <v>3.0840185421059419E-2</v>
       </c>
       <c r="O18" s="16">
         <f t="shared" si="6"/>
-        <v>21548.233852999918</v>
+        <v>-19582.105945260286</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="F19" s="5">
         <f t="shared" si="7"/>
-        <v>3530.3541660173346</v>
+        <v>0</v>
       </c>
       <c r="G19" s="5">
         <v>0</v>
@@ -4200,15 +4200,15 @@
       </c>
       <c r="M19" s="16">
         <f t="shared" si="8"/>
-        <v>55097.985203961616</v>
+        <v>12733.735211753599</v>
       </c>
       <c r="N19" s="17">
         <f t="shared" si="9"/>
-        <v>0.13229878188768052</v>
+        <v>3.0575667171113503E-2</v>
       </c>
       <c r="O19" s="16">
         <f t="shared" si="6"/>
-        <v>22565.110068589922</v>
+        <v>-19799.139923618095</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -4231,7 +4231,7 @@
       </c>
       <c r="F20" s="5">
         <f t="shared" si="7"/>
-        <v>3636.2647909978546</v>
+        <v>0</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -4258,15 +4258,15 @@
       </c>
       <c r="M20" s="16">
         <f t="shared" si="8"/>
-        <v>57260.084627385302</v>
+        <v>13624.907135411049</v>
       </c>
       <c r="N20" s="17">
         <f t="shared" si="9"/>
-        <v>0.12752826022473179</v>
+        <v>3.0345059983922843E-2</v>
       </c>
       <c r="O20" s="16">
         <f t="shared" si="6"/>
-        <v>23612.492570647613</v>
+        <v>-20022.68492132664</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="F21" s="5">
         <f t="shared" si="7"/>
-        <v>3745.3527347277904</v>
+        <v>0</v>
       </c>
       <c r="G21" s="5">
         <v>0</v>
@@ -4316,15 +4316,15 @@
       </c>
       <c r="M21" s="16">
         <f t="shared" si="8"/>
-        <v>59492.699134947885</v>
+        <v>14548.4663182144</v>
       </c>
       <c r="N21" s="17">
         <f t="shared" si="9"/>
-        <v>0.12326343452749274</v>
+        <v>3.0143092372106151E-2</v>
       </c>
       <c r="O21" s="16">
         <f t="shared" si="6"/>
-        <v>24691.296547767044</v>
+        <v>-20252.936268966441</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -4347,7 +4347,7 @@
       </c>
       <c r="F22" s="5">
         <f t="shared" si="7"/>
-        <v>3857.7133167696243</v>
+        <v>0</v>
       </c>
       <c r="G22" s="5">
         <v>0</v>
@@ -4374,15 +4374,15 @@
       </c>
       <c r="M22" s="16">
         <f t="shared" si="8"/>
-        <v>61798.174454507018</v>
+        <v>15505.614653271525</v>
       </c>
       <c r="N22" s="17">
         <f t="shared" si="9"/>
-        <v>0.1194287218429585</v>
+        <v>2.9965541147059092E-2</v>
       </c>
       <c r="O22" s="16">
         <f t="shared" si="6"/>
-        <v>25802.464644200059</v>
+        <v>-20490.095157035434</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -4405,7 +4405,7 @@
       </c>
       <c r="F23" s="5">
         <f t="shared" si="7"/>
-        <v>3973.4447162727133</v>
+        <v>0</v>
       </c>
       <c r="G23" s="5">
         <v>0</v>
@@ -4432,15 +4432,15 @@
       </c>
       <c r="M23" s="16">
         <f t="shared" si="8"/>
-        <v>64178.93606752799</v>
+        <v>16497.599472255428</v>
       </c>
       <c r="N23" s="17">
         <f t="shared" si="9"/>
-        <v>0.11596286008974531</v>
+        <v>2.9808983081378467E-2</v>
       </c>
       <c r="O23" s="16">
         <f t="shared" si="6"/>
-        <v>26946.967783526066</v>
+        <v>-20734.368811746495</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="F24" s="5">
         <f t="shared" si="7"/>
-        <v>4092.648057760895</v>
+        <v>0</v>
       </c>
       <c r="G24" s="5">
         <v>0</v>
@@ -4490,15 +4490,15 @@
       </c>
       <c r="M24" s="16">
         <f t="shared" si="8"/>
-        <v>66637.491983920641</v>
+        <v>17525.7152907899</v>
       </c>
       <c r="N24" s="17">
         <f t="shared" si="9"/>
-        <v>0.1128156692995725</v>
+        <v>2.9670613968504379E-2</v>
       </c>
       <c r="O24" s="16">
         <f t="shared" si="6"/>
-        <v>28125.806017031849</v>
+        <v>-20985.970676098892</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="F25" s="5">
         <f t="shared" si="7"/>
-        <v>4215.4274994937223</v>
+        <v>0</v>
       </c>
       <c r="G25" s="5">
         <v>0</v>
@@ -4548,15 +4548,15 @@
       </c>
       <c r="M25" s="16">
         <f t="shared" si="8"/>
-        <v>69176.435615692637</v>
+        <v>18591.305621767977</v>
       </c>
       <c r="N25" s="17">
         <f t="shared" si="9"/>
-        <v>0.10994565379980616</v>
+        <v>2.9548114663392747E-2</v>
       </c>
       <c r="O25" s="16">
         <f t="shared" si="6"/>
-        <v>29340.00939754281</v>
+        <v>-21245.120596381857</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -4579,7 +4579,7 @@
       </c>
       <c r="F26" s="5">
         <f t="shared" si="7"/>
-        <v>4341.8903244785342</v>
+        <v>0</v>
       </c>
       <c r="G26" s="5">
         <v>0</v>
@@ -4606,15 +4606,15 @@
       </c>
       <c r="M26" s="16">
         <f t="shared" si="8"/>
-        <v>71798.448753020231</v>
+        <v>19695.764859277817</v>
       </c>
       <c r="N26" s="17">
         <f t="shared" si="9"/>
-        <v>0.10731820116278989</v>
+        <v>2.9439550462907051E-2</v>
       </c>
       <c r="O26" s="16">
         <f t="shared" si="6"/>
-        <v>30590.638879469097</v>
+        <v>-21512.045014273313</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="F27" s="5">
         <f t="shared" si="7"/>
-        <v>4472.1470342128905</v>
+        <v>0</v>
       </c>
       <c r="G27" s="5">
         <v>0</v>
@@ -4664,15 +4664,15 @@
       </c>
       <c r="M27" s="16">
         <f t="shared" si="8"/>
-        <v>74506.304646467615</v>
+        <v>20840.540235912937</v>
       </c>
       <c r="N27" s="17">
         <f t="shared" si="9"/>
-        <v>0.10490421154690296</v>
+        <v>2.9343294531030073E-2</v>
       </c>
       <c r="O27" s="16">
         <f t="shared" si="6"/>
-        <v>31878.787245853171</v>
+        <v>-21786.977164701515</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -4695,7 +4695,7 @@
       </c>
       <c r="F28" s="5">
         <f t="shared" si="7"/>
-        <v>4606.3114452392774</v>
+        <v>0</v>
       </c>
       <c r="G28" s="5">
         <v>0</v>
@@ -4722,15 +4722,15 @@
       </c>
       <c r="M28" s="16">
         <f t="shared" si="8"/>
-        <v>77302.871199227913</v>
+        <v>22027.133856356581</v>
       </c>
       <c r="N28" s="17">
         <f t="shared" si="9"/>
-        <v>0.10267904203456556</v>
+        <v>2.9257968922122377E-2</v>
       </c>
       <c r="O28" s="16">
         <f t="shared" si="6"/>
-        <v>33205.580063228772</v>
+        <v>-22070.157279642561</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -4753,7 +4753,7 @@
       </c>
       <c r="F29" s="5">
         <f t="shared" si="7"/>
-        <v>4744.500788596456</v>
+        <v>0</v>
       </c>
       <c r="G29" s="5">
         <v>0</v>
@@ -4780,15 +4780,15 @@
       </c>
       <c r="M29" s="16">
         <f t="shared" si="8"/>
-        <v>80191.114273401196</v>
+        <v>23257.104810243727</v>
       </c>
       <c r="N29" s="17">
         <f t="shared" si="9"/>
-        <v>0.10062168462705127</v>
+        <v>2.9182398657987451E-2</v>
       </c>
       <c r="O29" s="16">
         <f t="shared" si="6"/>
-        <v>34572.176665125633</v>
+        <v>-22361.832798031835</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -4811,7 +4811,7 @@
       </c>
       <c r="F30" s="5">
         <f t="shared" si="7"/>
-        <v>4886.8358122543495</v>
+        <v>0</v>
       </c>
       <c r="G30" s="5">
         <v>0</v>
@@ -4838,15 +4838,15 @@
       </c>
       <c r="M30" s="16">
         <f t="shared" si="8"/>
-        <v>83174.101114474906</v>
+        <v>24532.071367422704</v>
       </c>
       <c r="N30" s="17">
         <f t="shared" si="9"/>
-        <v>9.8714119706590192E-2</v>
+        <v>2.9115575607861103E-2</v>
       </c>
       <c r="O30" s="16">
         <f t="shared" si="6"/>
-        <v>35979.771165079408</v>
+        <v>-22662.258581972794</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="F31" s="5">
         <f t="shared" si="7"/>
-        <v>5033.4408866219801</v>
+        <v>0</v>
       </c>
       <c r="G31" s="5">
         <v>0</v>
@@ -4896,15 +4896,15 @@
       </c>
       <c r="M31" s="16">
         <f t="shared" si="8"/>
-        <v>86255.003898326468</v>
+        <v>25853.713258862706</v>
       </c>
       <c r="N31" s="17">
         <f t="shared" si="9"/>
-        <v>9.6940802768885365E-2</v>
+        <v>2.9056629813906405E-2</v>
       </c>
       <c r="O31" s="16">
         <f t="shared" si="6"/>
-        <v>37429.593500031784</v>
+        <v>-22971.697139431977</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -4927,7 +4927,7 @@
       </c>
       <c r="F32" s="5">
         <f t="shared" si="7"/>
-        <v>5184.4441132206393</v>
+        <v>0</v>
       </c>
       <c r="G32" s="5">
         <v>0</v>
@@ -4954,15 +4954,15 @@
       </c>
       <c r="M32" s="16">
         <f t="shared" si="8"/>
-        <v>89437.103405231712</v>
+        <v>27223.77404658404</v>
       </c>
       <c r="N32" s="17">
         <f t="shared" si="9"/>
-        <v>9.5288253441250331E-2</v>
+        <v>2.9004806531183883E-2</v>
       </c>
       <c r="O32" s="16">
         <f t="shared" si="6"/>
-        <v>38922.910505032734</v>
+        <v>-23290.418853614938</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -4985,7 +4985,7 @@
       </c>
       <c r="F33" s="5">
         <f t="shared" si="7"/>
-        <v>5339.9774366172587</v>
+        <v>0</v>
       </c>
       <c r="G33" s="5">
         <v>0</v>
@@ -5005,15 +5005,15 @@
       </c>
       <c r="M33" s="16">
         <f t="shared" si="8"/>
-        <v>82481.950730477314</v>
+        <v>18402.221491070202</v>
       </c>
       <c r="N33" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828243E-2</v>
+        <v>1.8604838282208557E-2</v>
       </c>
       <c r="O33" s="16">
         <f t="shared" si="6"/>
-        <v>52808.667020183719</v>
+        <v>-11271.062219223384</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="F34" s="5">
         <f t="shared" si="7"/>
-        <v>5500.1767597157768</v>
+        <v>0</v>
       </c>
       <c r="G34" s="5">
         <v>0</v>
@@ -5056,15 +5056,15 @@
       </c>
       <c r="M34" s="16">
         <f t="shared" si="8"/>
-        <v>84956.409252391575</v>
+        <v>18954.288135802257</v>
       </c>
       <c r="N34" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828188E-2</v>
+        <v>1.8604838282208505E-2</v>
       </c>
       <c r="O34" s="16">
         <f t="shared" si="6"/>
-        <v>54392.927030789237</v>
+        <v>-11609.194085800087</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -5087,7 +5087,7 @@
       </c>
       <c r="F35" s="5">
         <f t="shared" si="7"/>
-        <v>5665.1820625072505</v>
+        <v>0</v>
       </c>
       <c r="G35" s="5">
         <v>0</v>
@@ -5107,15 +5107,15 @@
       </c>
       <c r="M35" s="16">
         <f t="shared" si="8"/>
-        <v>87505.101529963504</v>
+        <v>19522.91677987649</v>
       </c>
       <c r="N35" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828368E-2</v>
+        <v>1.8604838282208665E-2</v>
       </c>
       <c r="O35" s="16">
         <f t="shared" si="6"/>
-        <v>56024.714841712921</v>
+        <v>-11957.469908374091</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="F36" s="5">
         <f t="shared" si="7"/>
-        <v>5835.1375243824677</v>
+        <v>0</v>
       </c>
       <c r="G36" s="5">
         <v>0</v>
@@ -5158,15 +5158,15 @@
       </c>
       <c r="M36" s="16">
         <f t="shared" si="8"/>
-        <v>90130.254575862375</v>
+        <v>20108.604283272762</v>
       </c>
       <c r="N36" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828326E-2</v>
+        <v>1.860483828220864E-2</v>
       </c>
       <c r="O36" s="16">
         <f t="shared" si="6"/>
-        <v>57705.456286964305</v>
+        <v>-12316.194005625313</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="F37" s="5">
         <f t="shared" si="7"/>
-        <v>6010.1916501139422</v>
+        <v>0</v>
       </c>
       <c r="G37" s="5">
         <v>0</v>
@@ -5209,15 +5209,15 @@
       </c>
       <c r="M37" s="16">
         <f t="shared" si="8"/>
-        <v>92834.162213138159</v>
+        <v>20711.86241177085</v>
       </c>
       <c r="N37" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828243E-2</v>
+        <v>1.8604838282208554E-2</v>
       </c>
       <c r="O37" s="16">
         <f t="shared" si="6"/>
-        <v>59436.61997557323</v>
+        <v>-12685.679825794072</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -5240,7 +5240,7 @@
       </c>
       <c r="F38" s="5">
         <f t="shared" si="7"/>
-        <v>6190.4973996173603</v>
+        <v>0</v>
       </c>
       <c r="G38" s="5">
         <v>0</v>
@@ -5260,15 +5260,15 @@
       </c>
       <c r="M38" s="16">
         <f t="shared" si="8"/>
-        <v>95619.187079532392</v>
+        <v>21333.218284124068</v>
       </c>
       <c r="N38" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828326E-2</v>
+        <v>1.8604838282208637E-2</v>
       </c>
       <c r="O38" s="16">
         <f t="shared" si="6"/>
-        <v>61219.71857484043</v>
+        <v>-13066.250220567894</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -5291,7 +5291,7 @@
       </c>
       <c r="F39" s="5">
         <f t="shared" si="7"/>
-        <v>6376.2123216058817</v>
+        <v>0</v>
       </c>
       <c r="G39" s="5">
         <v>0</v>
@@ -5311,15 +5311,15 @@
       </c>
       <c r="M39" s="16">
         <f t="shared" si="8"/>
-        <v>98487.762691918353</v>
+        <v>21973.214832647784</v>
       </c>
       <c r="N39" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828313E-2</v>
+        <v>1.860483828220863E-2</v>
       </c>
       <c r="O39" s="16">
         <f t="shared" si="6"/>
-        <v>63056.310132085644</v>
+        <v>-13458.237727184931</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -5342,7 +5342,7 @@
       </c>
       <c r="F40" s="5">
         <f t="shared" si="7"/>
-        <v>6567.498691254058</v>
+        <v>0</v>
       </c>
       <c r="G40" s="5">
         <v>0</v>
@@ -5362,15 +5362,15 @@
       </c>
       <c r="M40" s="16">
         <f t="shared" si="8"/>
-        <v>101442.39557267599</v>
+        <v>22632.411277627285</v>
       </c>
       <c r="N40" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828368E-2</v>
+        <v>1.8604838282208686E-2</v>
       </c>
       <c r="O40" s="16">
         <f t="shared" si="6"/>
-        <v>64947.999436048223</v>
+        <v>-13861.98485900048</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="F41" s="5">
         <f t="shared" si="7"/>
-        <v>6764.5236519916798</v>
+        <v>0</v>
       </c>
       <c r="G41" s="5">
         <v>0</v>
@@ -5413,15 +5413,15 @@
       </c>
       <c r="M41" s="16">
         <f t="shared" si="8"/>
-        <v>104485.66743985613</v>
+        <v>23311.383615955976</v>
       </c>
       <c r="N41" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828257E-2</v>
+        <v>1.8604838282208581E-2</v>
       </c>
       <c r="O41" s="16">
         <f t="shared" si="6"/>
-        <v>66896.43941912966</v>
+        <v>-14277.844404770494</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="F42" s="5">
         <f t="shared" si="7"/>
-        <v>6967.4593615514304</v>
+        <v>0</v>
       </c>
       <c r="G42" s="5">
         <v>0</v>
@@ -5464,15 +5464,15 @@
       </c>
       <c r="M42" s="16">
         <f t="shared" si="8"/>
-        <v>107620.23746305177</v>
+        <v>24010.725124434604</v>
       </c>
       <c r="N42" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828229E-2</v>
+        <v>1.8604838282208543E-2</v>
       </c>
       <c r="O42" s="16">
         <f t="shared" si="6"/>
-        <v>68903.332601703558</v>
+        <v>-14706.179736913611</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -5495,7 +5495,7 @@
       </c>
       <c r="F43" s="5">
         <f t="shared" si="7"/>
-        <v>7176.4831423979731</v>
+        <v>0</v>
       </c>
       <c r="G43" s="5">
         <v>0</v>
@@ -5515,15 +5515,15 @@
       </c>
       <c r="M43" s="16">
         <f t="shared" si="8"/>
-        <v>110848.84458694332</v>
+        <v>24731.046878167639</v>
       </c>
       <c r="N43" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828215E-2</v>
+        <v>1.860483828220854E-2</v>
       </c>
       <c r="O43" s="16">
         <f t="shared" si="6"/>
-        <v>70970.432579754663</v>
+        <v>-15147.365129021018</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="F44" s="5">
         <f t="shared" si="7"/>
-        <v>7391.7776366699127</v>
+        <v>0</v>
       </c>
       <c r="G44" s="5">
         <v>0</v>
@@ -5566,15 +5566,15 @@
       </c>
       <c r="M44" s="16">
         <f t="shared" si="8"/>
-        <v>114174.30992455169</v>
+        <v>25472.978284512745</v>
       </c>
       <c r="N44" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828271E-2</v>
+        <v>1.8604838282208595E-2</v>
       </c>
       <c r="O44" s="16">
         <f t="shared" si="6"/>
-        <v>73099.545557147299</v>
+        <v>-15601.786082891649</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -5597,7 +5597,7 @@
       </c>
       <c r="F45" s="5">
         <f t="shared" si="7"/>
-        <v>7613.53096577001</v>
+        <v>0</v>
       </c>
       <c r="G45" s="5">
         <v>0</v>
@@ -5617,15 +5617,15 @@
       </c>
       <c r="M45" s="16">
         <f t="shared" si="8"/>
-        <v>117599.53922228819</v>
+        <v>26237.16763304807</v>
       </c>
       <c r="N45" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828243E-2</v>
+        <v>1.8604838282208554E-2</v>
       </c>
       <c r="O45" s="16">
         <f t="shared" si="6"/>
-        <v>75292.531923861723</v>
+        <v>-16069.8396653784</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -5648,7 +5648,7 @@
       </c>
       <c r="F46" s="5">
         <f t="shared" si="7"/>
-        <v>7841.9368947431103</v>
+        <v>0</v>
       </c>
       <c r="G46" s="5">
         <v>0</v>
@@ -5668,15 +5668,15 @@
       </c>
       <c r="M46" s="16">
         <f t="shared" si="8"/>
-        <v>121127.52539895702</v>
+        <v>27024.282662039685</v>
       </c>
       <c r="N46" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828368E-2</v>
+        <v>1.8604838282208675E-2</v>
       </c>
       <c r="O46" s="16">
         <f t="shared" si="6"/>
-        <v>77551.307881577581</v>
+        <v>-16551.934855339754</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
@@ -5699,7 +5699,7 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="7"/>
-        <v>8077.1950015854036</v>
+        <v>0</v>
       </c>
       <c r="G47" s="5">
         <v>0</v>
@@ -5719,15 +5719,15 @@
       </c>
       <c r="M47" s="16">
         <f t="shared" si="8"/>
-        <v>124761.35116092554</v>
+        <v>27835.011141900686</v>
       </c>
       <c r="N47" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828229E-2</v>
+        <v>1.8604838282208547E-2</v>
       </c>
       <c r="O47" s="16">
         <f t="shared" si="6"/>
-        <v>79877.847118024903</v>
+        <v>-17048.492900999947</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -5750,7 +5750,7 @@
       </c>
       <c r="F48" s="5">
         <f t="shared" si="7"/>
-        <v>8319.5108516329656</v>
+        <v>0</v>
       </c>
       <c r="G48" s="5">
         <v>0</v>
@@ -5770,15 +5770,15 @@
       </c>
       <c r="M48" s="16">
         <f t="shared" si="8"/>
-        <v>128504.19169575346</v>
+        <v>28670.061476157884</v>
       </c>
       <c r="N48" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828326E-2</v>
+        <v>1.8604838282208661E-2</v>
       </c>
       <c r="O48" s="16">
         <f t="shared" si="6"/>
-        <v>82274.182531565632</v>
+        <v>-17559.947688029941</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="F49" s="5">
         <f t="shared" si="7"/>
-        <v>8569.0961771819548</v>
+        <v>0</v>
       </c>
       <c r="G49" s="5">
         <v>0</v>
@@ -5821,15 +5821,15 @@
       </c>
       <c r="M49" s="16">
         <f t="shared" si="8"/>
-        <v>132359.31744662608</v>
+        <v>29530.163320442618</v>
       </c>
       <c r="N49" s="17">
         <f t="shared" si="9"/>
-        <v>8.339011435582834E-2</v>
+        <v>1.8604838282208658E-2</v>
       </c>
       <c r="O49" s="16">
         <f t="shared" si="6"/>
-        <v>84742.408007512611</v>
+        <v>-18086.746118670839</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
@@ -5852,7 +5852,7 @@
       </c>
       <c r="F50" s="5">
         <f t="shared" si="7"/>
-        <v>8826.1690624974144</v>
+        <v>0</v>
       </c>
       <c r="G50" s="5">
         <v>0</v>
@@ -5872,15 +5872,15 @@
       </c>
       <c r="M50" s="16">
         <f t="shared" si="8"/>
-        <v>136330.09697002475</v>
+        <v>30416.06822005576</v>
       </c>
       <c r="N50" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828257E-2</v>
+        <v>1.8604838282208574E-2</v>
       </c>
       <c r="O50" s="16">
         <f t="shared" si="6"/>
-        <v>87284.680247738012</v>
+        <v>-18629.348502230965</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="F51" s="5">
         <f t="shared" si="7"/>
-        <v>9090.9541343723376</v>
+        <v>0</v>
       </c>
       <c r="G51" s="5">
         <v>0</v>
@@ -5923,15 +5923,15 @@
       </c>
       <c r="M51" s="16">
         <f t="shared" si="8"/>
-        <v>140419.99987912562</v>
+        <v>31328.550266657574</v>
       </c>
       <c r="N51" s="17">
         <f t="shared" si="9"/>
-        <v>8.339011435582834E-2</v>
+        <v>1.8604838282208658E-2</v>
       </c>
       <c r="O51" s="16">
         <f t="shared" si="6"/>
-        <v>89903.220655170153</v>
+        <v>-19188.228957297895</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="F52" s="5">
         <f t="shared" si="7"/>
-        <v>9363.6827584035073</v>
+        <v>0</v>
       </c>
       <c r="G52" s="5">
         <v>0</v>
@@ -5974,15 +5974,15 @@
       </c>
       <c r="M52" s="16">
         <f t="shared" si="8"/>
-        <v>144632.59987549932</v>
+        <v>32268.406774657247</v>
       </c>
       <c r="N52" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828285E-2</v>
+        <v>1.8604838282208627E-2</v>
       </c>
       <c r="O52" s="16">
         <f t="shared" si="6"/>
-        <v>92600.317274825255</v>
+        <v>-19763.875826016832</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="F53" s="5">
         <f t="shared" si="7"/>
-        <v>9644.5932411556132</v>
+        <v>0</v>
       </c>
       <c r="G53" s="5">
         <v>0</v>
@@ -6025,15 +6025,15 @@
       </c>
       <c r="M53" s="16">
         <f t="shared" si="8"/>
-        <v>148971.57787176437</v>
+        <v>33236.458977897026</v>
       </c>
       <c r="N53" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828326E-2</v>
+        <v>1.8604838282208658E-2</v>
       </c>
       <c r="O53" s="16">
         <f t="shared" si="6"/>
-        <v>95378.326793070024</v>
+        <v>-20356.792100797338</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="F54" s="5">
         <f t="shared" si="7"/>
-        <v>9933.9310383902812</v>
+        <v>0</v>
       </c>
       <c r="G54" s="5">
         <v>0</v>
@@ -6076,15 +6076,15 @@
       </c>
       <c r="M54" s="16">
         <f t="shared" si="8"/>
-        <v>153440.72520791725</v>
+        <v>34233.552747233873</v>
       </c>
       <c r="N54" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828285E-2</v>
+        <v>1.8604838282208623E-2</v>
       </c>
       <c r="O54" s="16">
         <f t="shared" si="6"/>
-        <v>98239.676596862118</v>
+        <v>-20967.495863821256</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
@@ -6107,7 +6107,7 @@
       </c>
       <c r="F55" s="5">
         <f t="shared" si="7"/>
-        <v>10231.948969541991</v>
+        <v>0</v>
       </c>
       <c r="G55" s="5">
         <v>0</v>
@@ -6127,15 +6127,15 @@
       </c>
       <c r="M55" s="16">
         <f t="shared" si="8"/>
-        <v>158043.94696415483</v>
+        <v>35260.559329650969</v>
       </c>
       <c r="N55" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828326E-2</v>
+        <v>1.8604838282208665E-2</v>
       </c>
       <c r="O55" s="16">
         <f t="shared" si="6"/>
-        <v>101186.86689476798</v>
+        <v>-21596.520739735897</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
@@ -6158,7 +6158,7 @@
       </c>
       <c r="F56" s="5">
         <f t="shared" si="7"/>
-        <v>10538.90743862825</v>
+        <v>0</v>
       </c>
       <c r="G56" s="5">
         <v>0</v>
@@ -6178,15 +6178,15 @@
       </c>
       <c r="M56" s="16">
         <f t="shared" si="8"/>
-        <v>162785.26537307948</v>
+        <v>36318.376109540477</v>
       </c>
       <c r="N56" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828326E-2</v>
+        <v>1.8604838282208651E-2</v>
       </c>
       <c r="O56" s="16">
         <f t="shared" si="6"/>
-        <v>104222.47290161104</v>
+        <v>-22244.416361927975</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
@@ -6209,7 +6209,7 @@
       </c>
       <c r="F57" s="5">
         <f t="shared" si="7"/>
-        <v>10855.074661787097</v>
+        <v>0</v>
       </c>
       <c r="G57" s="5">
         <v>0</v>
@@ -6229,15 +6229,15 @@
       </c>
       <c r="M57" s="16">
         <f t="shared" si="8"/>
-        <v>167668.82333427167</v>
+        <v>37407.92739282651</v>
       </c>
       <c r="N57" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828215E-2</v>
+        <v>1.8604838282208561E-2</v>
       </c>
       <c r="O57" s="16">
         <f t="shared" si="6"/>
-        <v>107349.14708865936</v>
+        <v>-22911.748852785815</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -6260,7 +6260,7 @@
       </c>
       <c r="F58" s="5">
         <f t="shared" si="7"/>
-        <v>11180.72690164071</v>
+        <v>0</v>
       </c>
       <c r="G58" s="5">
         <v>0</v>
@@ -6280,15 +6280,15 @@
       </c>
       <c r="M58" s="16">
         <f t="shared" si="8"/>
-        <v>172698.88803429974</v>
+        <v>38530.165214611217</v>
       </c>
       <c r="N58" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828188E-2</v>
+        <v>1.8604838282208519E-2</v>
       </c>
       <c r="O58" s="16">
         <f t="shared" si="6"/>
-        <v>110569.62150131914</v>
+        <v>-23599.10131836939</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -6311,7 +6311,7 @@
       </c>
       <c r="F59" s="5">
         <f t="shared" si="7"/>
-        <v>11516.148708689932</v>
+        <v>0</v>
       </c>
       <c r="G59" s="5">
         <v>0</v>
@@ -6331,15 +6331,15 @@
       </c>
       <c r="M59" s="16">
         <f t="shared" si="8"/>
-        <v>177879.85467532882</v>
+        <v>39686.070171049651</v>
       </c>
       <c r="N59" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828229E-2</v>
+        <v>1.8604838282208564E-2</v>
       </c>
       <c r="O59" s="16">
         <f t="shared" si="6"/>
-        <v>113886.71014635872</v>
+        <v>-24307.074357920472</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
@@ -6362,7 +6362,7 @@
       </c>
       <c r="F60" s="5">
         <f t="shared" si="7"/>
-        <v>11861.63316995063</v>
+        <v>0</v>
       </c>
       <c r="G60" s="5">
         <v>0</v>
@@ -6382,15 +6382,15 @@
       </c>
       <c r="M60" s="16">
         <f t="shared" si="8"/>
-        <v>183216.25031558872</v>
+        <v>40876.652276181179</v>
       </c>
       <c r="N60" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828243E-2</v>
+        <v>1.8604838282208581E-2</v>
       </c>
       <c r="O60" s="16">
         <f t="shared" si="6"/>
-        <v>117303.31145074946</v>
+        <v>-25036.286588658084</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="F61" s="5">
         <f t="shared" si="7"/>
-        <v>12217.482165049149</v>
+        <v>0</v>
       </c>
       <c r="G61" s="5">
         <v>0</v>
@@ -6433,15 +6433,15 @@
       </c>
       <c r="M61" s="16">
         <f t="shared" si="8"/>
-        <v>188712.73782505642</v>
+        <v>42102.951844466617</v>
       </c>
       <c r="N61" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828257E-2</v>
+        <v>1.8604838282208585E-2</v>
       </c>
       <c r="O61" s="16">
         <f t="shared" si="6"/>
-        <v>120822.41079427196</v>
+        <v>-25787.375186317833</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
@@ -6464,7 +6464,7 @@
       </c>
       <c r="F62" s="5">
         <f t="shared" si="7"/>
-        <v>12584.006630000624</v>
+        <v>0</v>
       </c>
       <c r="G62" s="5">
         <v>0</v>
@@ -6484,15 +6484,15 @@
       </c>
       <c r="M62" s="16">
         <f t="shared" si="8"/>
-        <v>194374.11995980836</v>
+        <v>43366.04039980087</v>
       </c>
       <c r="N62" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828368E-2</v>
+        <v>1.8604838282208692E-2</v>
       </c>
       <c r="O62" s="16">
         <f t="shared" si="6"/>
-        <v>124447.08311810011</v>
+        <v>-26560.996441907366</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
@@ -6515,7 +6515,7 @@
       </c>
       <c r="F63" s="5">
         <f t="shared" si="7"/>
-        <v>12961.526828900644</v>
+        <v>0</v>
       </c>
       <c r="G63" s="5">
         <v>0</v>
@@ -6535,15 +6535,15 @@
       </c>
       <c r="M63" s="16">
         <f t="shared" si="8"/>
-        <v>200205.34355860221</v>
+        <v>44667.021611794495</v>
       </c>
       <c r="N63" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828188E-2</v>
+        <v>1.8604838282208522E-2</v>
       </c>
       <c r="O63" s="16">
         <f t="shared" si="6"/>
-        <v>128180.49561164314</v>
+        <v>-27357.826335164591</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
@@ -6566,7 +6566,7 @@
       </c>
       <c r="F64" s="5">
         <f t="shared" si="7"/>
-        <v>13350.372633767664</v>
+        <v>0</v>
       </c>
       <c r="G64" s="5">
         <v>0</v>
@@ -6586,15 +6586,15 @@
       </c>
       <c r="M64" s="16">
         <f t="shared" si="8"/>
-        <v>206211.50386536054</v>
+        <v>46007.03226014859</v>
       </c>
       <c r="N64" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828299E-2</v>
+        <v>1.860483828220863E-2</v>
       </c>
       <c r="O64" s="16">
         <f t="shared" si="6"/>
-        <v>132025.91047999242</v>
+        <v>-28178.56112521953</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
@@ -6617,7 +6617,7 @@
       </c>
       <c r="F65" s="5">
         <f t="shared" si="7"/>
-        <v>13750.883812780694</v>
+        <v>0</v>
       </c>
       <c r="G65" s="5">
         <v>0</v>
@@ -6637,15 +6637,15 @@
       </c>
       <c r="M65" s="16">
         <f t="shared" si="8"/>
-        <v>212397.84898132153</v>
+        <v>47387.243227953208</v>
       </c>
       <c r="N65" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828368E-2</v>
+        <v>1.8604838282208692E-2</v>
       </c>
       <c r="O65" s="16">
         <f t="shared" si="6"/>
-        <v>135986.6877943922</v>
+        <v>-29023.917958976115</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
@@ -6668,7 +6668,7 @@
       </c>
       <c r="F66" s="5">
         <f t="shared" si="7"/>
-        <v>14163.410327164114</v>
+        <v>0</v>
       </c>
       <c r="G66" s="5">
         <v>0</v>
@@ -6688,15 +6688,15 @@
       </c>
       <c r="M66" s="16">
         <f t="shared" si="8"/>
-        <v>218769.78445076087</v>
+        <v>48808.860524791482</v>
       </c>
       <c r="N66" s="17">
         <f t="shared" si="9"/>
-        <v>8.3390114355828243E-2</v>
+        <v>1.8604838282208568E-2</v>
       </c>
       <c r="O66" s="16">
         <f t="shared" si="6"/>
-        <v>140066.28842822398</v>
+        <v>-29894.635497745403</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>